<commit_message>
Modificado doParse en ExcelReadList
</commit_message>
<xml_diff>
--- a/src/test/resources/test7.xlsx
+++ b/src/test/resources/test7.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="5865"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="2640"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:G14"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -378,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -422,8 +422,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>

</xml_diff>